<commit_message>
Adding the code for Phase 2 modified before adding analysis
</commit_message>
<xml_diff>
--- a/project/phase1_results.xlsx
+++ b/project/phase1_results.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,19 +492,19 @@
         <v>3.158293710110962</v>
       </c>
       <c r="D2" t="n">
-        <v>6.11462159343153</v>
+        <v>6.049624213818273</v>
       </c>
       <c r="E2" t="n">
-        <v>3.18393426821774</v>
+        <v>3.173920439702034</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01892809485989577</v>
+        <v>-0.04606928475336147</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02564055810677779</v>
+        <v>0.01562672959107125</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03187022113277944</v>
+        <v>0.04864744263986305</v>
       </c>
       <c r="I2" t="n">
         <v>57</v>
@@ -521,19 +521,19 @@
         <v>1.132221084228233</v>
       </c>
       <c r="D3" t="n">
-        <v>1.345410699388109</v>
+        <v>1.439783477814177</v>
       </c>
       <c r="E3" t="n">
-        <v>1.151439237104154</v>
+        <v>1.251316609725247</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01762250789855146</v>
+        <v>0.1119952863246196</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01921815287592121</v>
+        <v>0.1190955254970143</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02607470392155561</v>
+        <v>0.163482991018465</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -550,22 +550,51 @@
         <v>8.302044618221775</v>
       </c>
       <c r="D4" t="n">
-        <v>7.397433846046987</v>
+        <v>7.474574587849915</v>
       </c>
       <c r="E4" t="n">
-        <v>8.188019710756839</v>
+        <v>8.261890110033912</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1087280675551927</v>
+        <v>-0.03158732575226431</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.1140249074649358</v>
+        <v>-0.0401545081878627</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1575546641539809</v>
+        <v>0.05108956523585606</v>
       </c>
       <c r="I4" t="n">
-        <v>74</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5.853086206137439</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6.835972487871987</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5.847429627558846</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6.824481192067192</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.005656578578593141</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.01149129580479524</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.01280807403511955</v>
+      </c>
+      <c r="I5" t="n">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,10 +638,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5.853086206137439</v>
+        <v>5.348999931723383</v>
       </c>
       <c r="C2" t="n">
-        <v>6.835972487871987</v>
+        <v>8.480579390302147</v>
       </c>
     </row>
     <row r="3">
@@ -620,10 +649,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>5.348999931723383</v>
+        <v>7.526828432972257</v>
       </c>
       <c r="C3" t="n">
-        <v>8.480579390302147</v>
+        <v>1.021908001361185</v>
       </c>
     </row>
     <row r="4">
@@ -631,10 +660,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>7.526828432972257</v>
+        <v>6.837243571439553</v>
       </c>
       <c r="C4" t="n">
-        <v>1.021908001361185</v>
+        <v>2.405244964820472</v>
       </c>
     </row>
     <row r="5">
@@ -642,10 +671,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>6.837243571439553</v>
+        <v>7.905431378799093</v>
       </c>
       <c r="C5" t="n">
-        <v>2.405244964820472</v>
+        <v>5.331689761992734</v>
       </c>
     </row>
     <row r="6">
@@ -653,10 +682,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7.905431378799093</v>
+        <v>3.397695124299078</v>
       </c>
       <c r="C6" t="n">
-        <v>5.331689761992734</v>
+        <v>4.381497769581268</v>
       </c>
     </row>
     <row r="7">
@@ -664,10 +693,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>3.397695124299078</v>
+        <v>1.226557369163704</v>
       </c>
       <c r="C7" t="n">
-        <v>4.381497769581268</v>
+        <v>1.994266211996512</v>
       </c>
     </row>
     <row r="8">
@@ -675,10 +704,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.226557369163704</v>
+        <v>6.364995317549043</v>
       </c>
       <c r="C8" t="n">
-        <v>1.994266211996512</v>
+        <v>6.177516092594001</v>
       </c>
     </row>
     <row r="9">
@@ -686,10 +715,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>6.364995317549043</v>
+        <v>5.923080891850031</v>
       </c>
       <c r="C9" t="n">
-        <v>6.177516092594001</v>
+        <v>4.069420434095067</v>
       </c>
     </row>
     <row r="10">
@@ -697,10 +726,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>5.923080891850031</v>
+        <v>8.977679486313688</v>
       </c>
       <c r="C10" t="n">
-        <v>4.069420434095067</v>
+        <v>8.846682710209841</v>
       </c>
     </row>
     <row r="11">
@@ -708,10 +737,120 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>8.977679486313688</v>
+        <v>2.08077204017929</v>
       </c>
       <c r="C11" t="n">
-        <v>8.846682710209841</v>
+        <v>6.771906721552654</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>5.202834579805807</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3.481935004471645</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>8.472348127649997</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.862361573672562</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4.13295200422529</v>
+      </c>
+      <c r="C14" t="n">
+        <v>8.122194816038338</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2.817260748267038</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.985497157488339</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1.672122748659079</v>
+      </c>
+      <c r="C16" t="n">
+        <v>7.661153181227182</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3.688936484365283</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2.202235735158713</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4.602714933194296</v>
+      </c>
+      <c r="C18" t="n">
+        <v>7.370594162298354</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.845137671949979</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.416170408515277</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1.726024364952975</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5.642659087894805</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.596123551745706</v>
+      </c>
+      <c r="C21" t="n">
+        <v>8.536904884051982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>